<commit_message>
updates, new tree, new filtering
</commit_message>
<xml_diff>
--- a/druhy.xlsx
+++ b/druhy.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,82 +437,68 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Oriolus_oriolus</t>
+          <t>Parus_major</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Parus_major</t>
+          <t>Phylloscopus_collybita</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Phylloscopus_collybita</t>
+          <t>Phylloscopus_sibilatrix</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Phylloscopus_sibilatrix</t>
+          <t>Poecile_palustris</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Poecile_palustris</t>
+          <t>Sitta_europaea</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Sitta_europaea</t>
+          <t>Sturnus_vulgaris</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sturnus_vulgaris</t>
+          <t>Sylvia_atricapilla</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sylvia_atricapilla</t>
+          <t>Troglodytes_troglodytes</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sylvia_borin</t>
+          <t>Turdus_merula</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
-        <is>
-          <t>Troglodytes_troglodytes</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Turdus_merula</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
         <is>
           <t>Turdus_philomelos</t>
         </is>

</xml_diff>